<commit_message>
add thumb field in bulk upload
</commit_message>
<xml_diff>
--- a/public/download/product_bulk_demo.xlsx
+++ b/public/download/product_bulk_demo.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>name</t>
   </si>
@@ -93,19 +94,28 @@
   </si>
   <si>
     <t>test,test1</t>
+  </si>
+  <si>
+    <t>thumbnail_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -139,19 +149,125 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="15" builtinId="5"/>
+    <cellStyle name="Currency" xfId="16" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
+    <cellStyle name="Comma" xfId="18" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -425,77 +541,81 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0d577574-df94-4c16-b0e9-9cc29956378e}">
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.428571428571429" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.285714285714285" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.571428571428571" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.571428571428573" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.142857142857142" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.571428571428573" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.142857142857142" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.428571428571429" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.142857142857142" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.142857142857142" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:16" ht="15" customHeight="1">
+      <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="P1" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -540,10 +660,13 @@
       </c>
       <c r="O2" t="s">
         <v>19</v>
+      </c>
+      <c r="P2">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup horizontalDpi="300" verticalDpi="300" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>